<commit_message>
Mise à jour du fichier d'évaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_HEIG-VD\7_5emeSemestre\TWEB\Project\Teaching-HEIGVD-TWEB-2015-Project\evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Documents\HEIG-VD\3eme\TWEB\Projet\Teaching-HEIGVD-TWEB-2015-Project\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -988,6 +988,9 @@
       <c r="B37">
         <v>1</v>
       </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -996,6 +999,9 @@
       <c r="B38">
         <v>1</v>
       </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -1054,7 +1060,7 @@
       </c>
       <c r="D44" s="3">
         <f>SUM(D34:D43)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,7 +1157,7 @@
       </c>
       <c r="D58" s="3">
         <f>SUM(D7,D21,D31,D44,D52)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>